<commit_message>
working on timepoint analysis
</commit_message>
<xml_diff>
--- a/RVD_Predictor_Analysis/results/ExcelFiles/H1N1_Only.xlsx
+++ b/RVD_Predictor_Analysis/results/ExcelFiles/H1N1_Only.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t xml:space="preserve">ABCG2</t>
   </si>
@@ -47,9 +47,6 @@
     <t xml:space="preserve">CD9</t>
   </si>
   <si>
-    <t xml:space="preserve">CFH</t>
-  </si>
-  <si>
     <t xml:space="preserve">CLEC5A</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t xml:space="preserve">RPL14</t>
   </si>
   <si>
-    <t xml:space="preserve">SDC2</t>
-  </si>
-  <si>
     <t xml:space="preserve">SGCD</t>
   </si>
   <si>
@@ -185,21 +179,39 @@
     <t xml:space="preserve">TTTY15</t>
   </si>
   <si>
+    <t xml:space="preserve">AGAP1</t>
+  </si>
+  <si>
     <t xml:space="preserve">ALPL</t>
   </si>
   <si>
+    <t xml:space="preserve">APOBEC3G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BTN3A2</t>
+  </si>
+  <si>
     <t xml:space="preserve">CD79B</t>
   </si>
   <si>
+    <t xml:space="preserve">ECHDC3</t>
+  </si>
+  <si>
     <t xml:space="preserve">ERO1B</t>
   </si>
   <si>
+    <t xml:space="preserve">FAM13A</t>
+  </si>
+  <si>
     <t xml:space="preserve">GALNT6</t>
   </si>
   <si>
     <t xml:space="preserve">GPM6A</t>
   </si>
   <si>
+    <t xml:space="preserve">HLA-DPA1</t>
+  </si>
+  <si>
     <t xml:space="preserve">HNRNPH1</t>
   </si>
   <si>
@@ -227,16 +239,22 @@
     <t xml:space="preserve">PRKAR2B</t>
   </si>
   <si>
+    <t xml:space="preserve">RUNX3</t>
+  </si>
+  <si>
     <t xml:space="preserve">SLC7A8</t>
   </si>
   <si>
     <t xml:space="preserve">SNORA21</t>
   </si>
   <si>
+    <t xml:space="preserve">SPATA20</t>
+  </si>
+  <si>
     <t xml:space="preserve">STRN3</t>
   </si>
   <si>
-    <t xml:space="preserve">YME1L1</t>
+    <t xml:space="preserve">TPP2</t>
   </si>
   <si>
     <t xml:space="preserve">ACAA2</t>
@@ -248,9 +266,15 @@
     <t xml:space="preserve">ACP2</t>
   </si>
   <si>
+    <t xml:space="preserve">ADM</t>
+  </si>
+  <si>
     <t xml:space="preserve">ALB</t>
   </si>
   <si>
+    <t xml:space="preserve">ASNS</t>
+  </si>
+  <si>
     <t xml:space="preserve">BPGM</t>
   </si>
   <si>
@@ -260,21 +284,36 @@
     <t xml:space="preserve">CALD1</t>
   </si>
   <si>
+    <t xml:space="preserve">CCND1</t>
+  </si>
+  <si>
     <t xml:space="preserve">CD28</t>
   </si>
   <si>
     <t xml:space="preserve">CDC25B</t>
   </si>
   <si>
+    <t xml:space="preserve">DGAT1</t>
+  </si>
+  <si>
     <t xml:space="preserve">DHFR</t>
   </si>
   <si>
     <t xml:space="preserve">DHX16</t>
   </si>
   <si>
+    <t xml:space="preserve">DLG5</t>
+  </si>
+  <si>
     <t xml:space="preserve">EBP</t>
   </si>
   <si>
+    <t xml:space="preserve">ENDOD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENO3</t>
+  </si>
+  <si>
     <t xml:space="preserve">ETV1</t>
   </si>
   <si>
@@ -341,6 +380,9 @@
     <t xml:space="preserve">PLOD2</t>
   </si>
   <si>
+    <t xml:space="preserve">PMPCA</t>
+  </si>
+  <si>
     <t xml:space="preserve">PPP2R5B</t>
   </si>
   <si>
@@ -353,6 +395,12 @@
     <t xml:space="preserve">RIOK3</t>
   </si>
   <si>
+    <t xml:space="preserve">SMTN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNCA</t>
+  </si>
+  <si>
     <t xml:space="preserve">SNRPA</t>
   </si>
   <si>
@@ -368,12 +416,30 @@
     <t xml:space="preserve">TSPAN5</t>
   </si>
   <si>
+    <t xml:space="preserve">XYLT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEX3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLEC10A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNTN5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENY2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FHL2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAMTOR2</t>
+  </si>
+  <si>
     <t xml:space="preserve">DOC2A</t>
   </si>
   <si>
-    <t xml:space="preserve">ECHDC3</t>
-  </si>
-  <si>
     <t xml:space="preserve">MARC1</t>
   </si>
   <si>
@@ -386,18 +452,12 @@
     <t xml:space="preserve">PRR5L</t>
   </si>
   <si>
-    <t xml:space="preserve">SPATA20</t>
-  </si>
-  <si>
     <t xml:space="preserve">TNFRSF21</t>
   </si>
   <si>
     <t xml:space="preserve">ACADVL</t>
   </si>
   <si>
-    <t xml:space="preserve">ADM</t>
-  </si>
-  <si>
     <t xml:space="preserve">CSF1</t>
   </si>
   <si>
@@ -443,7 +503,19 @@
     <t xml:space="preserve">VEGFA</t>
   </si>
   <si>
+    <t xml:space="preserve">ATP2A3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GZMH</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAPKAPK2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGS9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZSWIM8</t>
   </si>
 </sst>
 </file>
@@ -1495,6 +1567,126 @@
         <v>143</v>
       </c>
     </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>